<commit_message>
more test case for metric interface management.
</commit_message>
<xml_diff>
--- a/test-case/测试用例/测试用例.xlsx
+++ b/test-case/测试用例/测试用例.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\metric-sys\test-case\测试用例\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF19B984-DE8D-4202-A1FB-B1C24E226BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542128C2-E9CF-4338-9F53-EA1C7D05D7F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="599" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="599" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="使用说明" sheetId="5" r:id="rId1"/>
@@ -21,13 +21,15 @@
     <sheet name="指标数据查询分析" sheetId="8" r:id="rId6"/>
     <sheet name="系统首页" sheetId="7" r:id="rId7"/>
     <sheet name="系统管理" sheetId="10" r:id="rId8"/>
-    <sheet name="公共指标体系" sheetId="3" r:id="rId9"/>
-    <sheet name="卫健委指标体系" sheetId="4" r:id="rId10"/>
-    <sheet name="用户列表" sheetId="11" r:id="rId11"/>
-    <sheet name="机构信息表" sheetId="12" r:id="rId12"/>
+    <sheet name="指标接口维护" sheetId="13" r:id="rId9"/>
+    <sheet name="指标接口审批" sheetId="14" r:id="rId10"/>
+    <sheet name="公共指标体系" sheetId="3" r:id="rId11"/>
+    <sheet name="卫健委指标体系" sheetId="4" r:id="rId12"/>
+    <sheet name="用户列表" sheetId="11" r:id="rId13"/>
+    <sheet name="机构信息表" sheetId="12" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">机构信息表!$A$1:$D$2789</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">机构信息表!$A$1:$D$2789</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
@@ -292,8 +294,82 @@
 </comments>
 </file>
 
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Yu Xiao</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{98AB9BD4-39D3-42F4-B35F-F68D6FB8678E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Yu Xiao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+可以通过执行脚本校验或通过比对截图校验。
+如果使用脚本校验，需提供校验用脚本，以及脚本调用说明。
+如果通过截图对比校验，需要提供测试前及预期结果截图。
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Yu Xiao</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{925BB352-B223-4517-B990-77CA8CE0F140}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Yu Xiao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+可以通过执行脚本校验或通过比对截图校验。
+如果使用脚本校验，需提供校验用脚本，以及脚本调用说明。
+如果通过截图对比校验，需要提供测试前及预期结果截图。
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11976" uniqueCount="5673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12018" uniqueCount="5689">
   <si>
     <t>测试用例编号</t>
   </si>
@@ -21163,6 +21239,107 @@
     <t>在“已生效”标签页的指标目录列表中点击“人口基本情况”目录，该目录下的指标列表无变化。
 在“被拒绝”标签页的指标目录列表中点击“人口基本情况”目录，页面右侧列出被审批驳回的被移除指标。</t>
     <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-31-001</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>指标接口维护</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增指标接口</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>各项操作均提交成功</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>在“待审批”标签页打开新增的指标接口，各项属性与输入数据相符，该接口所含的各指标的筛选条件与设置的条件相符。</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-31-002</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改待审批指标接口</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、使用标准测试数据集
+2、执行用例3-31-001</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.使用admin用户或拥有【指标维护】权限的用户登录系统
+2.点击菜单 指标接口管理--&gt;指标接口维护
+3.点击页面左侧指标接口列表右侧的“新增”按钮，系统弹出指标接口配置窗口
+4.输入以下内容
+   接口代码：0002
+   接口名称：测试接口2
+   接口失效时间：2020-12-31
+   访问数据量阈值：99999
+   访问频次阈值： 100
+   申请备注：测试接口2
+5.点击窗口下方【确定】按钮
+6.点击页面左侧“待审批”标签
+7.点击“测试接口2”
+8.点击页面右侧“新增”按钮，系统显示指标列表。
+9.在指标列表中勾选”大专学历以上人口数量“，”累计新冠患者数量“，”就业人数“，点击“确定”。这三个指标被加入指标接口。
+10.点击“大专学历以上人口数量”指标右侧的“筛选条件“
+11.在“设置筛选条件”窗口中，点击“复杂查询”，在下方的查询条件输入框中，输入“d_date between '2020-01-01' and '2020-04-30'”，点击“保存”
+12.点击“就业人数”指标右侧的“筛选条件“
+13.在“设置筛选条件”窗口中，点击“简单查询”，在“村/社区”右侧的过滤条件输入框中，输入“='110101001001'”，点击“保存”</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.使用admin用户或拥有【指标维护】权限的用户登录系统
+2.点击菜单 指标接口管理--&gt;指标接口维护
+3.点击页面左侧“待审批”标签页，点击“测试接口2”右侧的编辑按钮，系统弹出指标接口配置窗口
+4.输入以下内容
+   申请备注：测试接口2备注
+5.点击窗口下方【确定】按钮
+6.点击页面左侧“待审批”标签，点击“测试接口2”
+7.在指标列表中勾选”累计新冠患者数量“，点击“删除”，该指标被从指标接口中删除。
+8.点击“大专学历以上人口数量”指标右侧的“筛选条件“
+9.在“设置筛选条件”窗口中，点击“复杂查询”，在下方的查询条件输入框中，输入“d_date between '2020-02-01' and '2020-04-30'”，点击“保存”
+10.点击“就业人数”指标右侧的“筛选条件“
+11.在“设置筛选条件”窗口中，点击“简单查询”，在“日期”右侧的过滤条件输入框中，输入“&lt; '2020-02-01'”，点击“保存”</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>在“待审批”标签页打开修改过的指标接口，各项属性与修改或的数据相符，该接口所含的各指标的筛选条件与修改过的条件相符。</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-32-001</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、使用标准测试数据集
+2、执行测试用例3-31-002</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.使用admin用户或拥有【指标维护】权限的用户登录系统
+2.点击菜单 指标接口管理--&gt;指标接口审批
+3.点击页面左侧“待审批”标签页
+4.点击“测试指标接口2”右侧的审批按钮
+5.填写审批意见：同意
+6.点击“提交”按钮
+</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>在“已生效”标签页中可以看到审批通过的指标接口，且指标接口所含指标与审批操作前相比没有变化。</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>审批通过新增指标接口</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -21591,12 +21768,6 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -21608,6 +21779,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -22027,6 +22204,206 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CEB32C-4CD7-4DCC-A4B3-437C5134071D}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="3" max="3" width="14.25" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="23.25" customWidth="1"/>
+    <col min="6" max="6" width="65.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.9140625" customWidth="1"/>
+    <col min="8" max="8" width="20.5" customWidth="1"/>
+    <col min="9" max="9" width="34.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="98">
+      <c r="A2" s="52" t="s">
+        <v>5684</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>5688</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>5685</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>5686</v>
+      </c>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52" t="s">
+        <v>5676</v>
+      </c>
+      <c r="I2" s="52" t="s">
+        <v>5687</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72745ED9-4FB7-44D6-9FC4-D66B36CB31A4}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="14.9140625" style="32" customWidth="1"/>
+    <col min="2" max="2" width="22.9140625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="20.25" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="32" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="31" customFormat="1" ht="15.5">
+      <c r="A1" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="33"/>
+      <c r="C5" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="33"/>
+      <c r="C7" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="33"/>
+      <c r="C8" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="33"/>
+      <c r="C9" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9DC77FF-A376-4934-BD20-E9C7927F74A0}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -22149,7 +22526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{628B8782-FF88-4718-8231-E340CD03B1BF}">
   <dimension ref="A1:F16"/>
   <sheetViews>
@@ -22447,7 +22824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41209079-642E-4F6B-82D8-AFD965546F83}">
   <dimension ref="A1:D2789"/>
   <sheetViews>
@@ -61522,8 +61899,8 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14"/>
@@ -61570,22 +61947,22 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="25" customFormat="1" ht="58" customHeight="1">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="58" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="26" t="s">
@@ -61596,12 +61973,12 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="25" customFormat="1">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
       <c r="H3" s="26" t="s">
         <v>10</v>
       </c>
@@ -62430,8 +62807,8 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14"/>
@@ -62529,7 +62906,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="210">
+    <row r="4" spans="1:9" ht="182">
       <c r="A4" s="37" t="s">
         <v>156</v>
       </c>
@@ -62555,7 +62932,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="210">
+    <row r="5" spans="1:9" ht="182">
       <c r="A5" s="37" t="s">
         <v>160</v>
       </c>
@@ -62581,7 +62958,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="182">
+    <row r="6" spans="1:9" ht="168">
       <c r="A6" s="37" t="s">
         <v>164</v>
       </c>
@@ -62607,7 +62984,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="70">
+    <row r="7" spans="1:9" ht="56">
       <c r="A7" s="37" t="s">
         <v>169</v>
       </c>
@@ -62656,7 +63033,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="378">
+    <row r="9" spans="1:9" ht="336">
       <c r="A9" s="37" t="s">
         <v>178</v>
       </c>
@@ -62682,7 +63059,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="210">
+    <row r="10" spans="1:9" ht="196">
       <c r="A10" s="37" t="s">
         <v>182</v>
       </c>
@@ -62708,7 +63085,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="182">
+    <row r="11" spans="1:9" ht="140">
       <c r="A11" s="37" t="s">
         <v>187</v>
       </c>
@@ -62734,7 +63111,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="126">
+    <row r="12" spans="1:9" ht="98">
       <c r="A12" s="37" t="s">
         <v>193</v>
       </c>
@@ -62760,7 +63137,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="182">
+    <row r="13" spans="1:9" ht="140">
       <c r="A13" s="40" t="s">
         <v>199</v>
       </c>
@@ -62787,7 +63164,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="140">
+    <row r="14" spans="1:9" ht="126">
       <c r="A14" s="37" t="s">
         <v>200</v>
       </c>
@@ -62813,7 +63190,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="70">
+    <row r="15" spans="1:9" ht="56">
       <c r="A15" s="28" t="s">
         <v>205</v>
       </c>
@@ -62839,7 +63216,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="70">
+    <row r="16" spans="1:9" ht="56">
       <c r="A16" s="28" t="s">
         <v>209</v>
       </c>
@@ -62865,7 +63242,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="70">
+    <row r="17" spans="1:9" ht="56">
       <c r="A17" s="28" t="s">
         <v>213</v>
       </c>
@@ -62891,7 +63268,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="70">
+    <row r="18" spans="1:9" ht="56">
       <c r="A18" s="28" t="s">
         <v>220</v>
       </c>
@@ -62983,22 +63360,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9A7C46-0EB5-4396-A7C3-F30946E192C4}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="14.75" style="58" customWidth="1"/>
-    <col min="2" max="2" width="13.4140625" style="58" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="58" customWidth="1"/>
-    <col min="4" max="4" width="21.08203125" style="58" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="58" customWidth="1"/>
-    <col min="6" max="6" width="58.58203125" style="58" customWidth="1"/>
-    <col min="7" max="7" width="20.9140625" style="58" customWidth="1"/>
-    <col min="8" max="8" width="34.1640625" style="58" customWidth="1"/>
-    <col min="9" max="9" width="30.4140625" style="58" customWidth="1"/>
-    <col min="10" max="16384" width="8.6640625" style="58"/>
+    <col min="1" max="1" width="14.75" style="56" customWidth="1"/>
+    <col min="2" max="2" width="13.4140625" style="56" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="56" customWidth="1"/>
+    <col min="4" max="4" width="21.08203125" style="56" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" style="56" customWidth="1"/>
+    <col min="6" max="6" width="58.58203125" style="56" customWidth="1"/>
+    <col min="7" max="7" width="20.9140625" style="56" customWidth="1"/>
+    <col min="8" max="8" width="34.1640625" style="56" customWidth="1"/>
+    <col min="9" max="9" width="30.4140625" style="56" customWidth="1"/>
+    <col min="10" max="16384" width="8.6640625" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.5">
@@ -63014,7 +63391,7 @@
       <c r="D1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="54" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="24" t="s">
@@ -63030,7 +63407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="112">
+    <row r="2" spans="1:9" ht="98">
       <c r="A2" s="47" t="s">
         <v>5624</v>
       </c>
@@ -63043,7 +63420,7 @@
       <c r="D2" s="47" t="s">
         <v>5634</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="55" t="s">
         <v>5626</v>
       </c>
       <c r="F2" s="47" t="s">
@@ -63070,7 +63447,7 @@
       <c r="D3" s="47" t="s">
         <v>5635</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="55" t="s">
         <v>5626</v>
       </c>
       <c r="F3" s="47" t="s">
@@ -63085,7 +63462,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="182">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="57" t="s">
         <v>5632</v>
       </c>
       <c r="B4" s="47" t="s">
@@ -63097,7 +63474,7 @@
       <c r="D4" s="47" t="s">
         <v>5633</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="55" t="s">
         <v>5636</v>
       </c>
       <c r="F4" s="47" t="s">
@@ -63123,7 +63500,7 @@
       <c r="D5" s="47" t="s">
         <v>5640</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="55" t="s">
         <v>5641</v>
       </c>
       <c r="F5" s="47" t="s">
@@ -63150,7 +63527,7 @@
       <c r="D6" s="47" t="s">
         <v>5645</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="55" t="s">
         <v>5641</v>
       </c>
       <c r="F6" s="47" t="s">
@@ -63177,7 +63554,7 @@
       <c r="D7" s="47" t="s">
         <v>5648</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="55" t="s">
         <v>5649</v>
       </c>
       <c r="F7" s="47" t="s">
@@ -63204,7 +63581,7 @@
       <c r="D8" s="47" t="s">
         <v>5653</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="55" t="s">
         <v>5649</v>
       </c>
       <c r="F8" s="47" t="s">
@@ -63231,7 +63608,7 @@
       <c r="D9" s="47" t="s">
         <v>5655</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="55" t="s">
         <v>5659</v>
       </c>
       <c r="F9" s="47" t="s">
@@ -63258,7 +63635,7 @@
       <c r="D10" s="47" t="s">
         <v>5663</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="55" t="s">
         <v>5659</v>
       </c>
       <c r="F10" s="47" t="s">
@@ -63285,7 +63662,7 @@
       <c r="D11" s="47" t="s">
         <v>5668</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="55" t="s">
         <v>5669</v>
       </c>
       <c r="F11" s="47" t="s">
@@ -63312,7 +63689,7 @@
       <c r="D12" s="47" t="s">
         <v>5663</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="55" t="s">
         <v>5669</v>
       </c>
       <c r="F12" s="47" t="s">
@@ -63337,8 +63714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02843B-15DE-4629-B690-383BE16AC9E1}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -63724,7 +64101,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -64012,119 +64389,111 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72745ED9-4FB7-44D6-9FC4-D66B36CB31A4}">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B75E71-A0AB-47EA-858C-994CF10C7BDF}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="14.9140625" style="32" customWidth="1"/>
-    <col min="2" max="2" width="22.9140625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="20.25" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="32" customWidth="1"/>
-    <col min="5" max="16384" width="8.6640625" style="32"/>
+    <col min="1" max="1" width="14.75" style="52" customWidth="1"/>
+    <col min="2" max="2" width="12.4140625" style="52" customWidth="1"/>
+    <col min="3" max="3" width="16.25" style="52" customWidth="1"/>
+    <col min="4" max="4" width="23.58203125" style="52" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" style="52" customWidth="1"/>
+    <col min="6" max="6" width="50.83203125" style="52" customWidth="1"/>
+    <col min="7" max="7" width="32.1640625" style="52" customWidth="1"/>
+    <col min="8" max="8" width="24.25" style="52" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" style="52" customWidth="1"/>
+    <col min="10" max="16384" width="8.6640625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="31" customFormat="1" ht="15.5">
-      <c r="A1" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3" s="34"/>
-      <c r="C3" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="33"/>
-      <c r="C5" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="B6" s="33"/>
-      <c r="C6" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7" s="33"/>
-      <c r="C7" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8" s="33"/>
-      <c r="C8" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="33"/>
-      <c r="C9" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>139</v>
+    <row r="1" spans="1:9" ht="15.5">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="350">
+      <c r="A2" s="52" t="s">
+        <v>5673</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>5675</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>5681</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>5676</v>
+      </c>
+      <c r="I2" s="52" t="s">
+        <v>5677</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="238">
+      <c r="A3" s="52" t="s">
+        <v>5678</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>5674</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>5679</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>5680</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>5682</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>5676</v>
+      </c>
+      <c r="I3" s="52" t="s">
+        <v>5683</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>